<commit_message>
add missing annotation value and further annotation analysis
</commit_message>
<xml_diff>
--- a/Datasets/annotated_dataset/tweets_session_2_3.xlsx
+++ b/Datasets/annotated_dataset/tweets_session_2_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nils_hellwig/Desktop/Studium/Masterstudium WS 2022:23/DH Projekt/Twitter_German_Federal_Election_Perception_2021/Datasets/annotated_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF88D9C-C4B7-814F-ACC0-75DE5E7B9D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D609C8F-7B68-7346-916E-B1645EF8018C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="21760" windowHeight="31640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7007" uniqueCount="4070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7008" uniqueCount="4070">
   <si>
     <t>id</t>
   </si>
@@ -12603,8 +12603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A473" workbookViewId="0">
-      <selection activeCell="F503" sqref="F503"/>
+    <sheetView tabSelected="1" topLeftCell="A881" workbookViewId="0">
+      <selection activeCell="E962" sqref="E962"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40203,6 +40203,9 @@
       <c r="D952" t="s">
         <v>3868</v>
       </c>
+      <c r="E952" t="s">
+        <v>4068</v>
+      </c>
       <c r="F952" t="s">
         <v>3869</v>
       </c>

</xml_diff>